<commit_message>
Summary:  - Change buttons in menu, from 2 different searches, to 1 search with option inside of it to screen the results - Only UI implemented  - UI:     - Chats --> All UI regarding Chats List, Chat buttons, inside each chat, ALL completed     - Posts --> Posts List design + Each Post design are completed  - UX:     - Chats + Posts --> most of the Ux fixed and improved duo to new UI workflow     - Fixed in most pages the margin and padding of parent layouts, in order to support all screen sizes, without overlapping on the AppBar nor the NavigationBar  - General:     - Edited and improved the PP slide of the Musician Finder Specification Document.pptx file     - Edited to show the curret state of the project of the Monday.com_Musician_Finder.xlsx file
Note:
    Monday.com free trial expired, so I converted it all to a Excel file and attached it to the project directory, I will update it each time someone start or finish working on one of the tasks

 #Lidor
</commit_message>
<xml_diff>
--- a/Monday.com_Musician_Finder.xlsx
+++ b/Monday.com_Musician_Finder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lidor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\P.Languages\GitHub\GitKraken\LocalReposetories\MusicianFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B99FEB8-5B0A-4E95-B2F6-B181E297A1BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FCC6EE-1EE4-474A-B947-5C06CF64577B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
   <si>
     <t>Musician Finder</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>General Chat Area</t>
-  </si>
-  <si>
-    <t>In Queue</t>
   </si>
   <si>
     <t>Chat Page</t>
@@ -219,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -249,12 +246,6 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF037F4C"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="1"/>
     </font>
@@ -333,7 +324,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,11 +373,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4ECCC6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF333333"/>
       </patternFill>
     </fill>
@@ -401,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -501,21 +487,6 @@
     </border>
     <border>
       <left style="thick">
-        <color rgb="FF4ECCC6"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF4ECCC6"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF4ECCC6"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF4ECCC6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
         <color rgb="FFFFF000"/>
       </left>
       <right style="thick">
@@ -548,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -586,22 +557,19 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -610,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -975,7 +943,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1108,7 @@
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1191,8 +1159,8 @@
       <c r="D12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>22</v>
+      <c r="E12" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="F12" s="1">
         <v>764011148</v>
@@ -1200,7 +1168,7 @@
     </row>
     <row r="13" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1211,8 +1179,8 @@
       <c r="D13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>18</v>
+      <c r="E13" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F13" s="1">
         <v>782138906</v>
@@ -1220,7 +1188,7 @@
     </row>
     <row r="14" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1231,8 +1199,8 @@
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>29</v>
+      <c r="E14" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="F14" s="1">
         <v>778647503</v>
@@ -1240,7 +1208,7 @@
     </row>
     <row r="15" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -1260,8 +1228,8 @@
     </row>
     <row r="16" spans="1:6" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:6" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>33</v>
+      <c r="A17" s="13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1286,16 +1254,16 @@
     </row>
     <row r="19" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>12</v>
@@ -1309,7 +1277,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
@@ -1331,8 +1299,8 @@
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>35</v>
+      <c r="C21" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>17</v>
@@ -1372,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
@@ -1386,13 +1354,13 @@
     </row>
     <row r="24" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>15</v>
@@ -1406,13 +1374,13 @@
     </row>
     <row r="25" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>
@@ -1426,7 +1394,7 @@
     </row>
     <row r="26" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
@@ -1446,10 +1414,10 @@
     </row>
     <row r="27" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
@@ -1472,13 +1440,13 @@
         <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>42</v>
+      <c r="E28" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="F28" s="1">
         <v>764011172</v>
@@ -1486,7 +1454,7 @@
     </row>
     <row r="29" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>14</v>
@@ -1506,13 +1474,13 @@
     </row>
     <row r="30" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>17</v>
@@ -1553,113 +1521,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>760037527</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
-        <v>760037527</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="D3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="18">
+        <v>0</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="18">
+        <v>796425954</v>
+      </c>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>760547484</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="19">
+      <c r="G4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="18">
         <v>0</v>
       </c>
-      <c r="I3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="19">
-        <v>796425954</v>
-      </c>
-      <c r="K3" s="19"/>
-    </row>
-    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
-        <v>760547484</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="19">
-        <v>0</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="19">
+      <c r="I4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="18">
         <v>796427178</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Summary:  - All UI and UX have been implemented and improved.  - Ready for punishment
Need Implementation:
 - Nothing :-)

Note:
    - Monday.com free trial expired, so I converted it all to a Excel file and attached it to the project directory, I will update it each time someone start or finish working on one of the tasks

 #Lidor
</commit_message>
<xml_diff>
--- a/Monday.com_Musician_Finder.xlsx
+++ b/Monday.com_Musician_Finder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\P.Languages\GitHub\GitKraken\LocalReposetories\MusicianFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FCC6EE-1EE4-474A-B947-5C06CF64577B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5A5BC6-4CB9-4A0F-8F97-8004B261F193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>Musician Finder</t>
   </si>
@@ -77,18 +77,12 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Publish Yourself</t>
   </si>
   <si>
     <t>Musician, Band</t>
   </si>
   <si>
-    <t>eliezerRevach</t>
-  </si>
-  <si>
     <t>Working on it</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
   </si>
   <si>
     <t>Instruments, Cities, Genres</t>
-  </si>
-  <si>
-    <t>Waiting for review</t>
   </si>
   <si>
     <t>Entrance Page</t>
@@ -206,17 +197,17 @@
 private int UserAge ;</t>
   </si>
   <si>
-    <t>Or Segal | yisrael</t>
-  </si>
-  <si>
     <t>General Search</t>
+  </si>
+  <si>
+    <t>Lidor | yisrael</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -280,21 +271,9 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFA25DDC"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="1"/>
     </font>
@@ -324,7 +303,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,11 +342,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00C875"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFDAB3D"/>
       </patternFill>
     </fill>
@@ -378,16 +352,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF579BFC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -457,21 +426,6 @@
     </border>
     <border>
       <left style="thick">
-        <color rgb="FF00B461"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF00B461"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF00B461"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF00B461"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
         <color rgb="FFE99729"/>
       </left>
       <right style="thick">
@@ -500,26 +454,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF4387E8"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF4387E8"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF4387E8"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF4387E8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,22 +493,16 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -578,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -942,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1048,19 +981,19 @@
     </row>
     <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
+      <c r="C7" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>22</v>
+      <c r="E7" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F7" s="1">
         <v>760321356</v>
@@ -1068,10 +1001,10 @@
     </row>
     <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -1088,10 +1021,10 @@
     </row>
     <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -1108,19 +1041,19 @@
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
+      <c r="C10" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>22</v>
+      <c r="E10" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="1">
         <v>760320604</v>
@@ -1128,7 +1061,7 @@
     </row>
     <row r="11" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -1148,7 +1081,7 @@
     </row>
     <row r="12" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
@@ -1159,8 +1092,8 @@
       <c r="D12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>18</v>
+      <c r="E12" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F12" s="1">
         <v>764011148</v>
@@ -1168,7 +1101,7 @@
     </row>
     <row r="13" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1188,7 +1121,7 @@
     </row>
     <row r="14" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1199,8 +1132,8 @@
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>18</v>
+      <c r="E14" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F14" s="1">
         <v>778647503</v>
@@ -1208,7 +1141,7 @@
     </row>
     <row r="15" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -1219,8 +1152,8 @@
       <c r="D15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>22</v>
+      <c r="E15" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="F15" s="1">
         <v>782138443</v>
@@ -1228,8 +1161,8 @@
     </row>
     <row r="16" spans="1:6" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:6" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>32</v>
+      <c r="A17" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1254,16 +1187,16 @@
     </row>
     <row r="19" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>12</v>
@@ -1277,7 +1210,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
@@ -1294,19 +1227,19 @@
     </row>
     <row r="21" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>34</v>
+      <c r="C21" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>18</v>
+      <c r="E21" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F21" s="1">
         <v>760326151</v>
@@ -1314,7 +1247,7 @@
     </row>
     <row r="22" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
@@ -1325,8 +1258,8 @@
       <c r="D22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>18</v>
+      <c r="E22" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F22" s="1">
         <v>760325403</v>
@@ -1334,13 +1267,13 @@
     </row>
     <row r="23" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
@@ -1354,19 +1287,19 @@
     </row>
     <row r="24" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>22</v>
+      <c r="E24" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F24" s="1">
         <v>760325690</v>
@@ -1374,13 +1307,13 @@
     </row>
     <row r="25" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>
@@ -1394,7 +1327,7 @@
     </row>
     <row r="26" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
@@ -1414,10 +1347,10 @@
     </row>
     <row r="27" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
@@ -1434,19 +1367,19 @@
     </row>
     <row r="28" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>41</v>
+      <c r="E28" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="F28" s="1">
         <v>764011172</v>
@@ -1454,7 +1387,7 @@
     </row>
     <row r="29" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>14</v>
@@ -1474,13 +1407,13 @@
     </row>
     <row r="30" spans="1:6" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>17</v>
@@ -1521,113 +1454,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="D2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="I2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="K2" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="17" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>760037527</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="D3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>760037527</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="H3" s="16">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="16">
+        <v>796425954</v>
+      </c>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>760547484</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="18">
+      <c r="H4" s="16">
         <v>0</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="18">
-        <v>796425954</v>
-      </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
-        <v>760547484</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="18">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="18">
+      <c r="I4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="16">
         <v>796427178</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>